<commit_message>
event study for systemic banking crisis
event study for systemic banking crisis, we did not found effect for this event.
</commit_message>
<xml_diff>
--- a/01-raw-data/IMF Crisis Data/SYSTEMIC BANKING CRISES DATABASE_2018.xlsx
+++ b/01-raw-data/IMF Crisis Data/SYSTEMIC BANKING CRISES DATABASE_2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{67E72F4F-82AD-4D6A-A812-AC0EE6B38C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84914DFA-6D37-4A8F-91C1-A0669BE2C97F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -9384,6 +9384,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -9717,9 +9721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -18455,7 +18459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BR51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>

</xml_diff>

<commit_message>
energy data from eam and other small changes
</commit_message>
<xml_diff>
--- a/01-raw-data/IMF Crisis Data/SYSTEMIC BANKING CRISES DATABASE_2018.xlsx
+++ b/01-raw-data/IMF Crisis Data/SYSTEMIC BANKING CRISES DATABASE_2018.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <xr:revisionPtr revIDLastSave="1" documentId="8_{67E72F4F-82AD-4D6A-A812-AC0EE6B38C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84914DFA-6D37-4A8F-91C1-A0669BE2C97F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="10" r:id="rId1"/>
@@ -9678,7 +9678,7 @@
   <dimension ref="A5:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9721,9 +9721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -18459,7 +18459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BR51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>

</xml_diff>